<commit_message>
feat: first util functions added
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dek2696\Programming\read-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dek2696\Programming\tmTurnover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D088E201-AF8D-42BA-B309-DC06E729A08F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF8EA3D-A8DB-42C8-8E84-0A6B34838159}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Denis</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Mega Khimki</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Lushnikova</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,6 +479,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45292</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>